<commit_message>
Alteracao para os dataSets ficarem com as colunas seguidas
</commit_message>
<xml_diff>
--- a/Testes/Dataset3/Populacao/statistic_average_fitness.xlsx
+++ b/Testes/Dataset3/Populacao/statistic_average_fitness.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrui2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1 - IPLeiria\2ºAno\2ºSemestre\Inteligência Artificial\Prática\Intellij Projects\StockingProblemProjectV4\Testes\Dataset3\Populacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D6B9CD-1F1D-42E5-B3A3-FBDDA2E42791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA97EC92-1FDE-4C56-B73E-C94DDCAFAF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statistic_average_fitness" sheetId="1" r:id="rId1"/>
@@ -594,48 +594,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Cor2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Cor3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Cor4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Cor5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Cor6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Cor1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Cor2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Cor3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Cor4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Cor5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Cor6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Cor1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Cor2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Cor3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Cor4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Cor5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Cor6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula Ligada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cor1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Cor2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Cor3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Cor4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Cor5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Cor6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Correto" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verificar Célula" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -653,7 +653,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -715,7 +715,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -766,7 +766,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -813,10 +813,10 @@
                     <c:v>Geração 625</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Geração 375</c:v>
+                    <c:v>Geração 500</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Geração 500</c:v>
+                    <c:v>Geração 375</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -830,10 +830,10 @@
                     <c:v>População 120</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>População 200</c:v>
+                    <c:v>População 150</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>População 150</c:v>
+                    <c:v>População 200</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -855,10 +855,10 @@
                   <c:v>92.14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.64</c:v>
+                  <c:v>88.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.7</c:v>
+                  <c:v>86.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -941,7 +941,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -979,7 +979,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="449405688"/>
@@ -1061,7 +1061,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1093,7 +1093,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="664896704"/>
@@ -1141,7 +1141,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1737,7 +1737,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2036,12 +2036,12 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2157,12 +2157,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -2180,18 +2180,18 @@
         <v>15</v>
       </c>
       <c r="I5">
-        <v>86.64</v>
+        <v>88.7</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2209,10 +2209,10 @@
         <v>15</v>
       </c>
       <c r="I6">
-        <v>88.7</v>
+        <v>86.64</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>